<commit_message>
Changed date and time fields for JGI app and verified database persistence
</commit_message>
<xml_diff>
--- a/app/tables/follow/forms/follow/follow.xlsx
+++ b/app/tables/follow/forms/follow/follow.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5900" yWindow="2860" windowWidth="30500" windowHeight="18040" tabRatio="500"/>
+    <workbookView xWindow="1360" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="55">
   <si>
     <t>clause</t>
   </si>
@@ -41,9 +41,6 @@
     <t>display.text</t>
   </si>
   <si>
-    <t>date</t>
-  </si>
-  <si>
     <t>FOL_date</t>
   </si>
   <si>
@@ -60,9 +57,6 @@
   </si>
   <si>
     <t>Community of focal chimp.</t>
-  </si>
-  <si>
-    <t>time</t>
   </si>
   <si>
     <t>FOL_time_begin</t>
@@ -600,7 +594,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -636,232 +630,232 @@
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>11</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="18" customHeight="1">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="C12" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="C13" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="C14" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="C15" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="C16" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="3:6">
       <c r="C17" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="3:6">
       <c r="C18" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="3:6">
       <c r="C19" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -889,10 +883,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C1" t="s">
         <v>5</v>
@@ -900,24 +894,24 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -947,27 +941,27 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>42</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C2" s="6"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B3" s="6">
         <v>20140715</v>
@@ -976,11 +970,11 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>